<commit_message>
refinements to metrics and plot outputs + new month run
</commit_message>
<xml_diff>
--- a/outputs/metric1_full.xlsx
+++ b/outputs/metric1_full.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,6 +420,23 @@
         <v>31.82</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D4">
+        <v>35.8</v>
+      </c>
+      <c r="E4">
+        <v>32.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -427,7 +444,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,6 +481,11 @@
           <t>CONCERN.HIGH</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>STATE.CODE</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +508,11 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>IN-AP</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -508,27 +535,37 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>IN-AP</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>Andhra Pradesh</t>
         </is>
       </c>
       <c r="B4">
         <v>2023</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>23.08</v>
       </c>
       <c r="F4">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>IN-AP</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -541,7 +578,7 @@
         <v>2023</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -552,55 +589,70 @@
       <c r="F5">
         <v>44</v>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>IN-AR</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="B6">
         <v>2023</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>39.39</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>24.24</v>
+        <v>44</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>IN-AR</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="B7">
         <v>2023</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>39.39</v>
+        <v>28</v>
       </c>
       <c r="F7">
-        <v>24.24</v>
+        <v>44</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>IN-AR</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B8">
@@ -613,16 +665,21 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>7.89</v>
+        <v>39.39</v>
       </c>
       <c r="F8">
-        <v>89.47</v>
+        <v>24.24</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>IN-AS</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B9">
@@ -635,104 +692,129 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>7.89</v>
+        <v>39.39</v>
       </c>
       <c r="F9">
-        <v>89.47</v>
+        <v>24.24</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>IN-AS</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B10">
         <v>2023</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>3.03</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>42.42</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>24.24</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>IN-AS</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>7.89</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>89.47</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>IN-BR</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B12">
         <v>2023</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>66.67</v>
+        <v>7.89</v>
       </c>
       <c r="F12">
-        <v>7.41</v>
+        <v>89.47</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>IN-BR</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B13">
         <v>2023</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>66.67</v>
+        <v>7.89</v>
       </c>
       <c r="F13">
-        <v>7.41</v>
+        <v>89.47</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>IN-BR</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B14">
@@ -750,11 +832,16 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>IN-CH</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B15">
@@ -772,99 +859,124 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>IN-CH</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B16">
         <v>2023</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F16">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>IN-CH</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B17">
         <v>2023</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="F17">
-        <v>50</v>
+        <v>7.41</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>IN-CT</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B18">
         <v>2023</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>54.55</v>
+        <v>66.67</v>
       </c>
       <c r="F18">
-        <v>45.45</v>
+        <v>7.41</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>IN-CT</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B19">
         <v>2023</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>63.64</v>
+        <v>66.67</v>
       </c>
       <c r="F19">
-        <v>45.45</v>
+        <v>7.41</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>IN-CT</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B20">
@@ -877,16 +989,21 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>30.3</v>
+        <v>100</v>
       </c>
       <c r="F20">
-        <v>3.03</v>
+        <v>0</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>IN-DN</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B21">
@@ -899,104 +1016,129 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>30.3</v>
+        <v>100</v>
       </c>
       <c r="F21">
-        <v>3.03</v>
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>IN-DN</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B22">
         <v>2023</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>54.55</v>
+        <v>100</v>
       </c>
       <c r="F22">
-        <v>27.27</v>
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>IN-DN</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B23">
         <v>2023</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>54.55</v>
+        <v>50</v>
       </c>
       <c r="F23">
-        <v>31.82</v>
+        <v>50</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>IN-DD</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B24">
         <v>2023</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>41.67</v>
+        <v>50</v>
       </c>
       <c r="F24">
-        <v>8.33</v>
+        <v>50</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>IN-DD</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B25">
         <v>2023</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>41.67</v>
+        <v>50</v>
       </c>
       <c r="F25">
-        <v>16.67</v>
+        <v>50</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>IN-DD</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B26">
@@ -1009,16 +1151,21 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>68.18000000000001</v>
+        <v>54.55</v>
       </c>
       <c r="F26">
-        <v>27.27</v>
+        <v>45.45</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>IN-DL</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B27">
@@ -1031,104 +1178,129 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>68.18000000000001</v>
+        <v>63.64</v>
       </c>
       <c r="F27">
-        <v>27.27</v>
+        <v>45.45</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>IN-DL</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B28">
         <v>2023</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>20.83</v>
+        <v>63.64</v>
       </c>
       <c r="F28">
-        <v>75</v>
+        <v>45.45</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>IN-DL</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B29">
         <v>2023</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>20.83</v>
+        <v>30.3</v>
       </c>
       <c r="F29">
-        <v>75</v>
+        <v>3.03</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>IN-GJ</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B30">
         <v>2023</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>16.67</v>
+        <v>30.3</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>3.03</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>IN-GJ</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B31">
         <v>2023</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>16.67</v>
+        <v>30.3</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>3.03</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>IN-GJ</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B32">
@@ -1141,16 +1313,21 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>50</v>
+        <v>54.55</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>27.27</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>IN-HR</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B33">
@@ -1163,104 +1340,129 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>50</v>
+        <v>54.55</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>31.82</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>IN-HR</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B34">
         <v>2023</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>48.08</v>
+        <v>54.55</v>
       </c>
       <c r="F34">
-        <v>30.77</v>
+        <v>31.82</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>IN-HR</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B35">
         <v>2023</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>50</v>
+        <v>41.67</v>
       </c>
       <c r="F35">
-        <v>30.77</v>
+        <v>8.33</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>IN-HP</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B36">
         <v>2023</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E36">
-        <v>27.78</v>
+        <v>41.67</v>
       </c>
       <c r="F36">
-        <v>2.78</v>
+        <v>16.67</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>IN-HP</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B37">
         <v>2023</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E37">
-        <v>27.78</v>
+        <v>41.67</v>
       </c>
       <c r="F37">
-        <v>2.78</v>
+        <v>16.67</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>IN-HP</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B38">
@@ -1273,16 +1475,21 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>31.25</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F38">
-        <v>56.25</v>
+        <v>27.27</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>IN-JK</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B39">
@@ -1295,104 +1502,129 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>31.25</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F39">
-        <v>56.25</v>
+        <v>27.27</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>IN-JK</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B40">
         <v>2023</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>9.09</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F40">
-        <v>63.64</v>
+        <v>27.27</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>IN-JK</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B41">
         <v>2023</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>9.09</v>
+        <v>20.83</v>
       </c>
       <c r="F41">
-        <v>63.64</v>
+        <v>75</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>IN-JH</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B42">
         <v>2023</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>27.27</v>
+        <v>20.83</v>
       </c>
       <c r="F42">
-        <v>54.55</v>
+        <v>75</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>IN-JH</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B43">
         <v>2023</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>27.27</v>
+        <v>20.83</v>
       </c>
       <c r="F43">
-        <v>54.55</v>
+        <v>75</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>IN-JH</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B44">
@@ -1405,16 +1637,21 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>45.45</v>
+        <v>16.67</v>
       </c>
       <c r="F44">
-        <v>36.36</v>
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>IN-KA</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B45">
@@ -1427,104 +1664,129 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>45.45</v>
+        <v>16.67</v>
       </c>
       <c r="F45">
-        <v>36.36</v>
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>IN-KA</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B46">
         <v>2023</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>56.67</v>
+        <v>16.67</v>
       </c>
       <c r="F46">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>IN-KA</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B47">
         <v>2023</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>56.67</v>
+        <v>50</v>
       </c>
       <c r="F47">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>IN-LA</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B48">
         <v>2023</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F48">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>IN-LA</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B49">
         <v>2023</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F49">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>IN-LA</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B50">
@@ -1537,16 +1799,21 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>31.82</v>
+        <v>48.08</v>
       </c>
       <c r="F50">
-        <v>63.64</v>
+        <v>30.77</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>IN-MP</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B51">
@@ -1556,107 +1823,132 @@
         <v>4</v>
       </c>
       <c r="D51">
-        <v>4.55</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>31.82</v>
+        <v>50</v>
       </c>
       <c r="F51">
-        <v>63.64</v>
+        <v>30.77</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>IN-MP</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B52">
         <v>2023</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>54.55</v>
+        <v>50</v>
       </c>
       <c r="F52">
-        <v>15.15</v>
+        <v>30.77</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>IN-MP</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B53">
         <v>2023</v>
       </c>
       <c r="C53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>54.55</v>
+        <v>27.78</v>
       </c>
       <c r="F53">
-        <v>15.15</v>
+        <v>2.78</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>IN-MH</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B54">
         <v>2023</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>18.92</v>
+        <v>27.78</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>2.78</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>IN-MH</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B55">
         <v>2023</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>18.92</v>
+        <v>27.78</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>2.78</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>IN-MH</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B56">
@@ -1669,16 +1961,21 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>42.42</v>
+        <v>31.25</v>
       </c>
       <c r="F56">
-        <v>33.33</v>
+        <v>56.25</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>IN-MN</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B57">
@@ -1691,104 +1988,129 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>42.42</v>
+        <v>31.25</v>
       </c>
       <c r="F57">
-        <v>33.33</v>
+        <v>56.25</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>IN-MN</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B58">
         <v>2023</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>50</v>
+        <v>31.25</v>
       </c>
       <c r="F58">
-        <v>50</v>
+        <v>62.5</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>IN-MN</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B59">
         <v>2023</v>
       </c>
       <c r="C59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>62.5</v>
+        <v>9.09</v>
       </c>
       <c r="F59">
-        <v>50</v>
+        <v>63.64</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>IN-ML</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B60">
         <v>2023</v>
       </c>
       <c r="C60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>33.33</v>
+        <v>9.09</v>
       </c>
       <c r="F60">
-        <v>62.67</v>
+        <v>63.64</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>IN-ML</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B61">
         <v>2023</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>33.33</v>
+        <v>9.09</v>
       </c>
       <c r="F61">
-        <v>62.67</v>
+        <v>63.64</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>IN-ML</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B62">
@@ -1801,16 +2123,21 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>7.69</v>
+        <v>27.27</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>54.55</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>IN-MZ</t>
+        </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B63">
@@ -1823,54 +2150,933 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>7.69</v>
+        <v>27.27</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>54.55</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>IN-MZ</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B64">
         <v>2023</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>43.48</v>
+        <v>27.27</v>
       </c>
       <c r="F64">
-        <v>13.04</v>
+        <v>81.81999999999999</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>IN-MZ</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
+          <t>Nagaland</t>
+        </is>
+      </c>
+      <c r="B65">
+        <v>2023</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>45.45</v>
+      </c>
+      <c r="F65">
+        <v>36.36</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>IN-NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Nagaland</t>
+        </is>
+      </c>
+      <c r="B66">
+        <v>2023</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>45.45</v>
+      </c>
+      <c r="F66">
+        <v>36.36</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>IN-NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Nagaland</t>
+        </is>
+      </c>
+      <c r="B67">
+        <v>2023</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>45.45</v>
+      </c>
+      <c r="F67">
+        <v>54.55</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>IN-NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="B68">
+        <v>2023</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>56.67</v>
+      </c>
+      <c r="F68">
+        <v>30</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>IN-OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="B69">
+        <v>2023</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>56.67</v>
+      </c>
+      <c r="F69">
+        <v>30</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>IN-OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>2023</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>56.67</v>
+      </c>
+      <c r="F70">
+        <v>33.33</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>IN-OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>2023</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>25</v>
+      </c>
+      <c r="F71">
+        <v>50</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>IN-PY</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>2023</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>25</v>
+      </c>
+      <c r="F72">
+        <v>50</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>IN-PY</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>2023</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>25</v>
+      </c>
+      <c r="F73">
+        <v>50</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>IN-PY</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>2023</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>31.82</v>
+      </c>
+      <c r="F74">
+        <v>63.64</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>IN-PB</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>2023</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <v>4.55</v>
+      </c>
+      <c r="E75">
+        <v>31.82</v>
+      </c>
+      <c r="F75">
+        <v>63.64</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>IN-PB</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>2023</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>4.55</v>
+      </c>
+      <c r="E76">
+        <v>31.82</v>
+      </c>
+      <c r="F76">
+        <v>63.64</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>IN-PB</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>2023</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>54.55</v>
+      </c>
+      <c r="F77">
+        <v>15.15</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>2023</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>54.55</v>
+      </c>
+      <c r="F78">
+        <v>15.15</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>2023</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>54.55</v>
+      </c>
+      <c r="F79">
+        <v>15.15</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>2023</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>18.92</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>2023</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>18.92</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>2023</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>18.92</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>2023</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>42.42</v>
+      </c>
+      <c r="F83">
+        <v>33.33</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>2023</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>42.42</v>
+      </c>
+      <c r="F84">
+        <v>33.33</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>2023</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>42.42</v>
+      </c>
+      <c r="F85">
+        <v>33.33</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>2023</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>50</v>
+      </c>
+      <c r="F86">
+        <v>50</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>2023</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>62.5</v>
+      </c>
+      <c r="F87">
+        <v>50</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>2023</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>62.5</v>
+      </c>
+      <c r="F88">
+        <v>50</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>2023</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>33.33</v>
+      </c>
+      <c r="F89">
+        <v>62.67</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>2023</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>33.33</v>
+      </c>
+      <c r="F90">
+        <v>62.67</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>2023</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>1.33</v>
+      </c>
+      <c r="E91">
+        <v>33.33</v>
+      </c>
+      <c r="F91">
+        <v>62.67</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>2023</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>7.69</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>2023</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>7.69</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>2023</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>7.69</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>West Bengal</t>
         </is>
       </c>
-      <c r="B65">
-        <v>2023</v>
-      </c>
-      <c r="C65">
-        <v>4</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
+      <c r="B95">
+        <v>2023</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
         <v>43.48</v>
       </c>
-      <c r="F65">
+      <c r="F95">
         <v>13.04</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>2023</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>43.48</v>
+      </c>
+      <c r="F96">
+        <v>13.04</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>2023</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
+      </c>
+      <c r="D97">
+        <v>4.35</v>
+      </c>
+      <c r="E97">
+        <v>43.48</v>
+      </c>
+      <c r="F97">
+        <v>13.04</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +3086,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1965,23 +3171,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Northeast</t>
+          <t>Magadha</t>
         </is>
       </c>
       <c r="B4">
         <v>2023</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>32.17</v>
+        <v>6.67</v>
       </c>
       <c r="F4">
-        <v>42.61</v>
+        <v>91.11</v>
       </c>
     </row>
     <row r="5">
@@ -1994,16 +3200,60 @@
         <v>2023</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>33.04</v>
+        <v>32.17</v>
       </c>
       <c r="F5">
         <v>42.61</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Northeast</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2023</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>33.04</v>
+      </c>
+      <c r="F6">
+        <v>42.61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Northeast</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>2023</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.87</v>
+      </c>
+      <c r="E7">
+        <v>34.78</v>
+      </c>
+      <c r="F7">
+        <v>47.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix to data import script + premature rerun of analysis (before pulling)
</commit_message>
<xml_diff>
--- a/outputs/metric1_full.xlsx
+++ b/outputs/metric1_full.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,16 +408,16 @@
         <v>2023</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>0.27</v>
+        <v>1.23</v>
       </c>
       <c r="D3">
-        <v>35.53</v>
+        <v>36.21</v>
       </c>
       <c r="E3">
-        <v>31.82</v>
+        <v>32.78</v>
       </c>
     </row>
     <row r="4">
@@ -425,16 +425,16 @@
         <v>2023</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0.6899999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="D4">
-        <v>35.8</v>
+        <v>35.53</v>
       </c>
       <c r="E4">
-        <v>32.78</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="5">
@@ -442,15 +442,32 @@
         <v>2023</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D5">
+        <v>35.8</v>
+      </c>
+      <c r="E5">
+        <v>32.78</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>1.23</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>36.08</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>32.78</v>
       </c>
     </row>
@@ -461,7 +478,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -541,7 +558,7 @@
         <v>2023</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -568,7 +585,7 @@
         <v>2023</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -595,7 +612,7 @@
         <v>2023</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -615,27 +632,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>Andhra Pradesh</t>
         </is>
       </c>
       <c r="B6">
         <v>2023</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>23.08</v>
       </c>
       <c r="F6">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>IN-AR</t>
+          <t>IN-AP</t>
         </is>
       </c>
     </row>
@@ -649,7 +666,7 @@
         <v>2023</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -676,7 +693,7 @@
         <v>2023</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -703,13 +720,13 @@
         <v>2023</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>44</v>
@@ -723,54 +740,54 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="B10">
         <v>2023</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>39.39</v>
+        <v>28</v>
       </c>
       <c r="F10">
-        <v>24.24</v>
+        <v>44</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>IN-AS</t>
+          <t>IN-AR</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>39.39</v>
+        <v>28</v>
       </c>
       <c r="F11">
-        <v>24.24</v>
+        <v>44</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>IN-AS</t>
+          <t>IN-AR</t>
         </is>
       </c>
     </row>
@@ -784,13 +801,13 @@
         <v>2023</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>3.03</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>42.42</v>
+        <v>39.39</v>
       </c>
       <c r="F12">
         <v>24.24</v>
@@ -811,7 +828,7 @@
         <v>2023</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>3.03</v>
@@ -831,81 +848,81 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B14">
         <v>2023</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>7.89</v>
+        <v>39.39</v>
       </c>
       <c r="F14">
-        <v>89.47</v>
+        <v>24.24</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>IN-BR</t>
+          <t>IN-AS</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B15">
         <v>2023</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>3.03</v>
       </c>
       <c r="E15">
-        <v>7.89</v>
+        <v>42.42</v>
       </c>
       <c r="F15">
-        <v>89.47</v>
+        <v>24.24</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>IN-BR</t>
+          <t>IN-AS</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="B16">
         <v>2023</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3.03</v>
       </c>
       <c r="E16">
-        <v>7.89</v>
+        <v>42.42</v>
       </c>
       <c r="F16">
-        <v>89.47</v>
+        <v>24.24</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>IN-BR</t>
+          <t>IN-AS</t>
         </is>
       </c>
     </row>
@@ -919,7 +936,7 @@
         <v>2023</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -939,7 +956,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B18">
@@ -952,21 +969,21 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>7.89</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>89.47</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>IN-CH</t>
+          <t>IN-BR</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B19">
@@ -979,21 +996,21 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>7.89</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>89.47</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>IN-CH</t>
+          <t>IN-BR</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B20">
@@ -1006,21 +1023,21 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>7.89</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>89.47</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>IN-CH</t>
+          <t>IN-BR</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="B21">
@@ -1033,21 +1050,21 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>7.89</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>89.47</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>IN-CH</t>
+          <t>IN-BR</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B22">
@@ -1060,109 +1077,109 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="F22">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>IN-CT</t>
+          <t>IN-CH</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B23">
         <v>2023</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="F23">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>IN-CT</t>
+          <t>IN-CH</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B24">
         <v>2023</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="F24">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>IN-CT</t>
+          <t>IN-CH</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B25">
         <v>2023</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="F25">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>IN-CT</t>
+          <t>IN-CH</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chandigarh</t>
         </is>
       </c>
       <c r="B26">
         <v>2023</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1175,311 +1192,311 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>IN-DN</t>
+          <t>IN-CH</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B27">
         <v>2023</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>66.67</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>7.41</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>IN-DN</t>
+          <t>IN-CT</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B28">
         <v>2023</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>66.67</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>7.41</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>IN-DN</t>
+          <t>IN-CT</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B29">
         <v>2023</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>66.67</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>7.41</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>IN-DN</t>
+          <t>IN-CT</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B30">
         <v>2023</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="F30">
-        <v>50</v>
+        <v>7.41</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-CT</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="B31">
         <v>2023</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="F31">
-        <v>50</v>
+        <v>7.41</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-CT</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B32">
         <v>2023</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-DN</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B33">
         <v>2023</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-DN</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B34">
         <v>2023</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>54.55</v>
+        <v>100</v>
       </c>
       <c r="F34">
-        <v>45.45</v>
+        <v>0</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-DN</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B35">
         <v>2023</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>63.64</v>
+        <v>100</v>
       </c>
       <c r="F35">
-        <v>45.45</v>
+        <v>0</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-DN</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Dadra and Nagar Haveli</t>
         </is>
       </c>
       <c r="B36">
         <v>2023</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>63.64</v>
+        <v>100</v>
       </c>
       <c r="F36">
-        <v>45.45</v>
+        <v>0</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-DN</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B37">
         <v>2023</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>63.64</v>
+        <v>50</v>
       </c>
       <c r="F37">
-        <v>45.45</v>
+        <v>50</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-DD</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B38">
@@ -1492,21 +1509,21 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>30.3</v>
+        <v>50</v>
       </c>
       <c r="F38">
-        <v>3.03</v>
+        <v>50</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>IN-GJ</t>
+          <t>IN-DD</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B39">
@@ -1519,21 +1536,21 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>30.3</v>
+        <v>50</v>
       </c>
       <c r="F39">
-        <v>3.03</v>
+        <v>50</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>IN-GJ</t>
+          <t>IN-DD</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B40">
@@ -1546,21 +1563,21 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>30.3</v>
+        <v>50</v>
       </c>
       <c r="F40">
-        <v>3.03</v>
+        <v>50</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>IN-GJ</t>
+          <t>IN-DD</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="B41">
@@ -1570,24 +1587,24 @@
         <v>6</v>
       </c>
       <c r="D41">
-        <v>3.03</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>30.3</v>
+        <v>50</v>
       </c>
       <c r="F41">
-        <v>3.03</v>
+        <v>50</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>IN-GJ</t>
+          <t>IN-DD</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B42">
@@ -1603,423 +1620,423 @@
         <v>54.55</v>
       </c>
       <c r="F42">
-        <v>27.27</v>
+        <v>45.45</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-DL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B43">
         <v>2023</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>54.55</v>
+        <v>63.64</v>
       </c>
       <c r="F43">
-        <v>31.82</v>
+        <v>45.45</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-DL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B44">
         <v>2023</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>54.55</v>
+        <v>63.64</v>
       </c>
       <c r="F44">
-        <v>31.82</v>
+        <v>45.45</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-DL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B45">
         <v>2023</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>54.55</v>
+        <v>63.64</v>
       </c>
       <c r="F45">
-        <v>31.82</v>
+        <v>45.45</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-DL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B46">
         <v>2023</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>41.67</v>
+        <v>63.64</v>
       </c>
       <c r="F46">
-        <v>8.33</v>
+        <v>45.45</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-DL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B47">
         <v>2023</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>41.67</v>
+        <v>30.3</v>
       </c>
       <c r="F47">
-        <v>16.67</v>
+        <v>3.03</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-GJ</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B48">
         <v>2023</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>8.33</v>
+        <v>3.03</v>
       </c>
       <c r="E48">
-        <v>41.67</v>
+        <v>30.3</v>
       </c>
       <c r="F48">
-        <v>16.67</v>
+        <v>3.03</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-GJ</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B49">
         <v>2023</v>
       </c>
       <c r="C49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D49">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>41.67</v>
+        <v>30.3</v>
       </c>
       <c r="F49">
-        <v>16.67</v>
+        <v>3.03</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-GJ</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B50">
         <v>2023</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>68.18000000000001</v>
+        <v>30.3</v>
       </c>
       <c r="F50">
-        <v>27.27</v>
+        <v>3.03</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-GJ</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="B51">
         <v>2023</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>3.03</v>
       </c>
       <c r="E51">
-        <v>68.18000000000001</v>
+        <v>30.3</v>
       </c>
       <c r="F51">
-        <v>27.27</v>
+        <v>3.03</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-GJ</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B52">
         <v>2023</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>68.18000000000001</v>
+        <v>54.55</v>
       </c>
       <c r="F52">
         <v>27.27</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-HR</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B53">
         <v>2023</v>
       </c>
       <c r="C53">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>68.18000000000001</v>
+        <v>54.55</v>
       </c>
       <c r="F53">
-        <v>27.27</v>
+        <v>31.82</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-HR</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B54">
         <v>2023</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>20.83</v>
+        <v>54.55</v>
       </c>
       <c r="F54">
-        <v>75</v>
+        <v>31.82</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-HR</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B55">
         <v>2023</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>20.83</v>
+        <v>54.55</v>
       </c>
       <c r="F55">
-        <v>75</v>
+        <v>31.82</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-HR</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="B56">
         <v>2023</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>20.83</v>
+        <v>54.55</v>
       </c>
       <c r="F56">
-        <v>75</v>
+        <v>31.82</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-HR</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B57">
         <v>2023</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>20.83</v>
+        <v>41.67</v>
       </c>
       <c r="F57">
-        <v>75</v>
+        <v>8.33</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-HP</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B58">
@@ -2029,24 +2046,24 @@
         <v>3</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E58">
+        <v>41.67</v>
+      </c>
+      <c r="F58">
         <v>16.67</v>
       </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>IN-KA</t>
+          <t>IN-HP</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B59">
@@ -2056,24 +2073,24 @@
         <v>4</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E59">
+        <v>41.67</v>
+      </c>
+      <c r="F59">
         <v>16.67</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>IN-KA</t>
+          <t>IN-HP</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B60">
@@ -2083,24 +2100,24 @@
         <v>5</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E60">
+        <v>41.67</v>
+      </c>
+      <c r="F60">
         <v>16.67</v>
       </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>IN-KA</t>
+          <t>IN-HP</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="B61">
@@ -2110,24 +2127,24 @@
         <v>6</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="E61">
+        <v>41.67</v>
+      </c>
+      <c r="F61">
         <v>16.67</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>IN-KA</t>
+          <t>IN-HP</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B62">
@@ -2140,426 +2157,426 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>50</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>27.27</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>IN-LA</t>
+          <t>IN-JK</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B63">
         <v>2023</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>50</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>27.27</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>IN-LA</t>
+          <t>IN-JK</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B64">
         <v>2023</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>50</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>27.27</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>IN-LA</t>
+          <t>IN-JK</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B65">
         <v>2023</v>
       </c>
       <c r="C65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>50</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>27.27</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>IN-LA</t>
+          <t>IN-JK</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="B66">
         <v>2023</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>48.08</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F66">
-        <v>30.77</v>
+        <v>27.27</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-JK</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B67">
         <v>2023</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>50</v>
+        <v>20.83</v>
       </c>
       <c r="F67">
-        <v>30.77</v>
+        <v>75</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-JH</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B68">
         <v>2023</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
       <c r="E68">
-        <v>50</v>
+        <v>20.83</v>
       </c>
       <c r="F68">
-        <v>30.77</v>
+        <v>75</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-JH</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B69">
         <v>2023</v>
       </c>
       <c r="C69">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>51.92</v>
+        <v>20.83</v>
       </c>
       <c r="F69">
-        <v>30.77</v>
+        <v>75</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-JH</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B70">
         <v>2023</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>27.78</v>
+        <v>20.83</v>
       </c>
       <c r="F70">
-        <v>2.78</v>
+        <v>75</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>IN-MH</t>
+          <t>IN-JH</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="B71">
         <v>2023</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>27.78</v>
+        <v>20.83</v>
       </c>
       <c r="F71">
-        <v>2.78</v>
+        <v>75</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>IN-MH</t>
+          <t>IN-JH</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B72">
         <v>2023</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>27.78</v>
+        <v>16.67</v>
       </c>
       <c r="F72">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>IN-MH</t>
+          <t>IN-KA</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B73">
         <v>2023</v>
       </c>
       <c r="C73">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>27.78</v>
+        <v>16.67</v>
       </c>
       <c r="F73">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>IN-MH</t>
+          <t>IN-KA</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B74">
         <v>2023</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>31.25</v>
+        <v>16.67</v>
       </c>
       <c r="F74">
-        <v>56.25</v>
+        <v>0</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-KA</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B75">
         <v>2023</v>
       </c>
       <c r="C75">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>31.25</v>
+        <v>16.67</v>
       </c>
       <c r="F75">
-        <v>56.25</v>
+        <v>0</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-KA</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B76">
         <v>2023</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>31.25</v>
+        <v>16.67</v>
       </c>
       <c r="F76">
-        <v>62.5</v>
+        <v>0</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-KA</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B77">
         <v>2023</v>
       </c>
       <c r="C77">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>31.25</v>
+        <v>50</v>
       </c>
       <c r="F77">
-        <v>62.5</v>
+        <v>0</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-LA</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B78">
@@ -2572,21 +2589,21 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>9.09</v>
+        <v>50</v>
       </c>
       <c r="F78">
-        <v>63.64</v>
+        <v>0</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-LA</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B79">
@@ -2599,21 +2616,21 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>9.09</v>
+        <v>50</v>
       </c>
       <c r="F79">
-        <v>63.64</v>
+        <v>0</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-LA</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B80">
@@ -2626,21 +2643,21 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>9.09</v>
+        <v>50</v>
       </c>
       <c r="F80">
-        <v>63.64</v>
+        <v>0</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-LA</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Ladakh</t>
         </is>
       </c>
       <c r="B81">
@@ -2653,21 +2670,21 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>9.09</v>
+        <v>50</v>
       </c>
       <c r="F81">
-        <v>63.64</v>
+        <v>0</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-LA</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B82">
@@ -2680,426 +2697,426 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>27.27</v>
+        <v>48.08</v>
       </c>
       <c r="F82">
-        <v>54.55</v>
+        <v>30.77</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-MP</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B83">
         <v>2023</v>
       </c>
       <c r="C83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="E83">
-        <v>27.27</v>
+        <v>51.92</v>
       </c>
       <c r="F83">
-        <v>54.55</v>
+        <v>30.77</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-MP</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B84">
         <v>2023</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D84">
         <v>0</v>
       </c>
       <c r="E84">
-        <v>27.27</v>
+        <v>50</v>
       </c>
       <c r="F84">
-        <v>81.81999999999999</v>
+        <v>30.77</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-MP</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B85">
         <v>2023</v>
       </c>
       <c r="C85">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="E85">
-        <v>27.27</v>
+        <v>50</v>
       </c>
       <c r="F85">
-        <v>81.81999999999999</v>
+        <v>30.77</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-MP</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="B86">
         <v>2023</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>45.45</v>
+        <v>51.92</v>
       </c>
       <c r="F86">
-        <v>36.36</v>
+        <v>30.77</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-MP</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B87">
         <v>2023</v>
       </c>
       <c r="C87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87">
-        <v>45.45</v>
+        <v>27.78</v>
       </c>
       <c r="F87">
-        <v>36.36</v>
+        <v>2.78</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-MH</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B88">
         <v>2023</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>45.45</v>
+        <v>27.78</v>
       </c>
       <c r="F88">
-        <v>54.55</v>
+        <v>2.78</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-MH</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B89">
         <v>2023</v>
       </c>
       <c r="C89">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="E89">
-        <v>45.45</v>
+        <v>27.78</v>
       </c>
       <c r="F89">
-        <v>54.55</v>
+        <v>2.78</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-MH</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B90">
         <v>2023</v>
       </c>
       <c r="C90">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
       <c r="E90">
-        <v>56.67</v>
+        <v>27.78</v>
       </c>
       <c r="F90">
-        <v>30</v>
+        <v>2.78</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-MH</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="B91">
         <v>2023</v>
       </c>
       <c r="C91">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>56.67</v>
+        <v>27.78</v>
       </c>
       <c r="F91">
-        <v>30</v>
+        <v>2.78</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-MH</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B92">
         <v>2023</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
       <c r="E92">
-        <v>56.67</v>
+        <v>31.25</v>
       </c>
       <c r="F92">
-        <v>33.33</v>
+        <v>56.25</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-MN</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B93">
         <v>2023</v>
       </c>
       <c r="C93">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>56.67</v>
+        <v>31.25</v>
       </c>
       <c r="F93">
-        <v>33.33</v>
+        <v>62.5</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-MN</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B94">
         <v>2023</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>25</v>
+        <v>31.25</v>
       </c>
       <c r="F94">
-        <v>50</v>
+        <v>56.25</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>IN-PY</t>
+          <t>IN-MN</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B95">
         <v>2023</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
       <c r="E95">
-        <v>25</v>
+        <v>31.25</v>
       </c>
       <c r="F95">
-        <v>50</v>
+        <v>62.5</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>IN-PY</t>
+          <t>IN-MN</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="B96">
         <v>2023</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
       <c r="E96">
-        <v>25</v>
+        <v>31.25</v>
       </c>
       <c r="F96">
-        <v>50</v>
+        <v>62.5</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>IN-PY</t>
+          <t>IN-MN</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B97">
         <v>2023</v>
       </c>
       <c r="C97">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>25</v>
+        <v>9.09</v>
       </c>
       <c r="F97">
-        <v>50</v>
+        <v>63.64</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>IN-PY</t>
+          <t>IN-ML</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B98">
@@ -3112,21 +3129,21 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>31.82</v>
+        <v>9.09</v>
       </c>
       <c r="F98">
         <v>63.64</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-ML</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B99">
@@ -3136,24 +3153,24 @@
         <v>4</v>
       </c>
       <c r="D99">
-        <v>4.55</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>31.82</v>
+        <v>9.09</v>
       </c>
       <c r="F99">
         <v>63.64</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-ML</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B100">
@@ -3163,24 +3180,24 @@
         <v>5</v>
       </c>
       <c r="D100">
-        <v>4.55</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>31.82</v>
+        <v>9.09</v>
       </c>
       <c r="F100">
         <v>63.64</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-ML</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="B101">
@@ -3190,24 +3207,24 @@
         <v>6</v>
       </c>
       <c r="D101">
-        <v>4.55</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>36.36</v>
+        <v>9.09</v>
       </c>
       <c r="F101">
         <v>63.64</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-ML</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B102">
@@ -3220,426 +3237,426 @@
         <v>0</v>
       </c>
       <c r="E102">
+        <v>27.27</v>
+      </c>
+      <c r="F102">
         <v>54.55</v>
       </c>
-      <c r="F102">
-        <v>15.15</v>
-      </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-MZ</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B103">
         <v>2023</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
-        <v>54.55</v>
+        <v>27.27</v>
       </c>
       <c r="F103">
-        <v>15.15</v>
+        <v>81.81999999999999</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-MZ</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B104">
         <v>2023</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="E104">
+        <v>27.27</v>
+      </c>
+      <c r="F104">
         <v>54.55</v>
       </c>
-      <c r="F104">
-        <v>15.15</v>
-      </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-MZ</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B105">
         <v>2023</v>
       </c>
       <c r="C105">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D105">
-        <v>6.06</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>54.55</v>
+        <v>27.27</v>
       </c>
       <c r="F105">
-        <v>15.15</v>
+        <v>81.81999999999999</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-MZ</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="B106">
         <v>2023</v>
       </c>
       <c r="C106">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
       <c r="E106">
-        <v>18.92</v>
+        <v>27.27</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>81.81999999999999</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>IN-TN</t>
+          <t>IN-MZ</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="B107">
         <v>2023</v>
       </c>
       <c r="C107">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107">
-        <v>18.92</v>
+        <v>45.45</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>36.36</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>IN-TN</t>
+          <t>IN-NL</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="B108">
         <v>2023</v>
       </c>
       <c r="C108">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108">
-        <v>18.92</v>
+        <v>45.45</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>54.55</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>IN-TN</t>
+          <t>IN-NL</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="B109">
         <v>2023</v>
       </c>
       <c r="C109">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
       <c r="E109">
-        <v>18.92</v>
+        <v>45.45</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>36.36</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>IN-TN</t>
+          <t>IN-NL</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="B110">
         <v>2023</v>
       </c>
       <c r="C110">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D110">
         <v>0</v>
       </c>
       <c r="E110">
-        <v>42.42</v>
+        <v>45.45</v>
       </c>
       <c r="F110">
-        <v>33.33</v>
+        <v>54.55</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-NL</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="B111">
         <v>2023</v>
       </c>
       <c r="C111">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
       <c r="E111">
-        <v>42.42</v>
+        <v>45.45</v>
       </c>
       <c r="F111">
-        <v>33.33</v>
+        <v>54.55</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-NL</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B112">
         <v>2023</v>
       </c>
       <c r="C112">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D112">
         <v>0</v>
       </c>
       <c r="E112">
-        <v>42.42</v>
+        <v>56.67</v>
       </c>
       <c r="F112">
-        <v>33.33</v>
+        <v>30</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-OR</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B113">
         <v>2023</v>
       </c>
       <c r="C113">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
       <c r="E113">
-        <v>42.42</v>
+        <v>56.67</v>
       </c>
       <c r="F113">
         <v>33.33</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-OR</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B114">
         <v>2023</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
       <c r="E114">
-        <v>50</v>
+        <v>56.67</v>
       </c>
       <c r="F114">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>IN-TR</t>
+          <t>IN-OR</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B115">
         <v>2023</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
       <c r="E115">
-        <v>62.5</v>
+        <v>56.67</v>
       </c>
       <c r="F115">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>IN-TR</t>
+          <t>IN-OR</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B116">
         <v>2023</v>
       </c>
       <c r="C116">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
       <c r="E116">
-        <v>62.5</v>
+        <v>56.67</v>
       </c>
       <c r="F116">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>IN-TR</t>
+          <t>IN-OR</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="B117">
         <v>2023</v>
       </c>
       <c r="C117">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
       <c r="E117">
-        <v>62.5</v>
+        <v>25</v>
       </c>
       <c r="F117">
         <v>50</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>IN-TR</t>
+          <t>IN-PY</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="B118">
@@ -3652,21 +3669,21 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="F118">
-        <v>62.67</v>
+        <v>50</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>IN-UP</t>
+          <t>IN-PY</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="B119">
@@ -3679,21 +3696,21 @@
         <v>0</v>
       </c>
       <c r="E119">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="F119">
-        <v>62.67</v>
+        <v>50</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>IN-UP</t>
+          <t>IN-PY</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="B120">
@@ -3703,24 +3720,24 @@
         <v>5</v>
       </c>
       <c r="D120">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="F120">
-        <v>62.67</v>
+        <v>50</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>IN-UP</t>
+          <t>IN-PY</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="B121">
@@ -3730,24 +3747,24 @@
         <v>6</v>
       </c>
       <c r="D121">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="F121">
-        <v>62.67</v>
+        <v>50</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>IN-UP</t>
+          <t>IN-PY</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="B122">
@@ -3760,201 +3777,1065 @@
         <v>0</v>
       </c>
       <c r="E122">
-        <v>7.69</v>
+        <v>31.82</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>63.64</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>IN-UL</t>
+          <t>IN-PB</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="B123">
         <v>2023</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="E123">
-        <v>7.69</v>
+        <v>36.36</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>63.64</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>IN-UL</t>
+          <t>IN-PB</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="B124">
         <v>2023</v>
       </c>
       <c r="C124">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="E124">
-        <v>7.69</v>
+        <v>31.82</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>63.64</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>IN-UL</t>
+          <t>IN-PB</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="B125">
         <v>2023</v>
       </c>
       <c r="C125">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="E125">
-        <v>7.69</v>
+        <v>31.82</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>63.64</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>IN-UL</t>
+          <t>IN-PB</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="B126">
         <v>2023</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="E126">
-        <v>43.48</v>
+        <v>36.36</v>
       </c>
       <c r="F126">
-        <v>13.04</v>
+        <v>63.64</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>IN-WB</t>
+          <t>IN-PB</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="B127">
         <v>2023</v>
       </c>
       <c r="C127">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
       <c r="E127">
-        <v>43.48</v>
+        <v>54.55</v>
       </c>
       <c r="F127">
-        <v>13.04</v>
+        <v>15.15</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>IN-WB</t>
+          <t>IN-RJ</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="B128">
         <v>2023</v>
       </c>
       <c r="C128">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D128">
-        <v>4.35</v>
+        <v>6.06</v>
       </c>
       <c r="E128">
-        <v>43.48</v>
+        <v>54.55</v>
       </c>
       <c r="F128">
-        <v>13.04</v>
+        <v>15.15</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>IN-WB</t>
+          <t>IN-RJ</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B129">
+        <v>2023</v>
+      </c>
+      <c r="C129">
+        <v>4</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>54.55</v>
+      </c>
+      <c r="F129">
+        <v>15.15</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B130">
+        <v>2023</v>
+      </c>
+      <c r="C130">
+        <v>5</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>54.55</v>
+      </c>
+      <c r="F130">
+        <v>15.15</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B131">
+        <v>2023</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+      <c r="D131">
+        <v>6.06</v>
+      </c>
+      <c r="E131">
+        <v>54.55</v>
+      </c>
+      <c r="F131">
+        <v>15.15</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B132">
+        <v>2023</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>18.92</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B133">
+        <v>2023</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>18.92</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B134">
+        <v>2023</v>
+      </c>
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>18.92</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B135">
+        <v>2023</v>
+      </c>
+      <c r="C135">
+        <v>5</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>18.92</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B136">
+        <v>2023</v>
+      </c>
+      <c r="C136">
+        <v>6</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>18.92</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>IN-TN</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B137">
+        <v>2023</v>
+      </c>
+      <c r="C137">
+        <v>3</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>42.42</v>
+      </c>
+      <c r="F137">
+        <v>33.33</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B138">
+        <v>2023</v>
+      </c>
+      <c r="C138">
+        <v>3</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>42.42</v>
+      </c>
+      <c r="F138">
+        <v>33.33</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B139">
+        <v>2023</v>
+      </c>
+      <c r="C139">
+        <v>4</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>42.42</v>
+      </c>
+      <c r="F139">
+        <v>33.33</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B140">
+        <v>2023</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>42.42</v>
+      </c>
+      <c r="F140">
+        <v>33.33</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B141">
+        <v>2023</v>
+      </c>
+      <c r="C141">
+        <v>6</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>42.42</v>
+      </c>
+      <c r="F141">
+        <v>33.33</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B142">
+        <v>2023</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>50</v>
+      </c>
+      <c r="F142">
+        <v>50</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B143">
+        <v>2023</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>62.5</v>
+      </c>
+      <c r="F143">
+        <v>50</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B144">
+        <v>2023</v>
+      </c>
+      <c r="C144">
+        <v>4</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>62.5</v>
+      </c>
+      <c r="F144">
+        <v>50</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B145">
+        <v>2023</v>
+      </c>
+      <c r="C145">
+        <v>5</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>62.5</v>
+      </c>
+      <c r="F145">
+        <v>50</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B146">
+        <v>2023</v>
+      </c>
+      <c r="C146">
+        <v>6</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>62.5</v>
+      </c>
+      <c r="F146">
+        <v>50</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>IN-TR</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B147">
+        <v>2023</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>33.33</v>
+      </c>
+      <c r="F147">
+        <v>62.67</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B148">
+        <v>2023</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>1.33</v>
+      </c>
+      <c r="E148">
+        <v>33.33</v>
+      </c>
+      <c r="F148">
+        <v>62.67</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B149">
+        <v>2023</v>
+      </c>
+      <c r="C149">
+        <v>4</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>33.33</v>
+      </c>
+      <c r="F149">
+        <v>62.67</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B150">
+        <v>2023</v>
+      </c>
+      <c r="C150">
+        <v>5</v>
+      </c>
+      <c r="D150">
+        <v>1.33</v>
+      </c>
+      <c r="E150">
+        <v>33.33</v>
+      </c>
+      <c r="F150">
+        <v>62.67</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B151">
+        <v>2023</v>
+      </c>
+      <c r="C151">
+        <v>6</v>
+      </c>
+      <c r="D151">
+        <v>1.33</v>
+      </c>
+      <c r="E151">
+        <v>33.33</v>
+      </c>
+      <c r="F151">
+        <v>62.67</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>IN-UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B152">
+        <v>2023</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>7.69</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B153">
+        <v>2023</v>
+      </c>
+      <c r="C153">
+        <v>3</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>7.69</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B154">
+        <v>2023</v>
+      </c>
+      <c r="C154">
+        <v>4</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>7.69</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B155">
+        <v>2023</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>7.69</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B156">
+        <v>2023</v>
+      </c>
+      <c r="C156">
+        <v>6</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>7.69</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>IN-UL</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
           <t>West Bengal</t>
         </is>
       </c>
-      <c r="B129">
-        <v>2023</v>
-      </c>
-      <c r="C129">
+      <c r="B157">
+        <v>2023</v>
+      </c>
+      <c r="C157">
+        <v>3</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>43.48</v>
+      </c>
+      <c r="F157">
+        <v>13.04</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B158">
+        <v>2023</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+      <c r="D158">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E158">
+        <v>47.83</v>
+      </c>
+      <c r="F158">
+        <v>13.04</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B159">
+        <v>2023</v>
+      </c>
+      <c r="C159">
+        <v>4</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>43.48</v>
+      </c>
+      <c r="F159">
+        <v>13.04</v>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B160">
+        <v>2023</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+      <c r="D160">
+        <v>4.35</v>
+      </c>
+      <c r="E160">
+        <v>43.48</v>
+      </c>
+      <c r="F160">
+        <v>13.04</v>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>IN-WB</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B161">
+        <v>2023</v>
+      </c>
+      <c r="C161">
         <v>6</v>
       </c>
-      <c r="D129">
+      <c r="D161">
         <v>8.699999999999999</v>
       </c>
-      <c r="E129">
+      <c r="E161">
         <v>43.48</v>
       </c>
-      <c r="F129">
+      <c r="F161">
         <v>13.04</v>
       </c>
-      <c r="G129" t="inlineStr">
+      <c r="G161" t="inlineStr">
         <is>
           <t>IN-WB</t>
         </is>
@@ -3967,7 +4848,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4037,7 +4918,7 @@
         <v>2023</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4059,7 +4940,7 @@
         <v>2023</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -4081,7 +4962,7 @@
         <v>2023</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4096,23 +4977,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Northeast</t>
+          <t>Magadha</t>
         </is>
       </c>
       <c r="B6">
         <v>2023</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>32.17</v>
+        <v>6.67</v>
       </c>
       <c r="F6">
-        <v>42.61</v>
+        <v>91.11</v>
       </c>
     </row>
     <row r="7">
@@ -4125,13 +5006,13 @@
         <v>2023</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>33.04</v>
+        <v>32.17</v>
       </c>
       <c r="F7">
         <v>42.61</v>
@@ -4147,7 +5028,7 @@
         <v>2023</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0.87</v>
@@ -4169,15 +5050,59 @@
         <v>2023</v>
       </c>
       <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>33.04</v>
+      </c>
+      <c r="F9">
+        <v>42.61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Northeast</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0.87</v>
+      </c>
+      <c r="E10">
+        <v>34.78</v>
+      </c>
+      <c r="F10">
+        <v>47.83</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Northeast</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>2023</v>
+      </c>
+      <c r="C11">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>0.87</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>34.78</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>47.83</v>
       </c>
     </row>

</xml_diff>